<commit_message>
auto.py interface output issue fixed
</commit_message>
<xml_diff>
--- a/snap_in.xlsx
+++ b/snap_in.xlsx
@@ -85,9 +85,6 @@
     <t>self</t>
   </si>
   <si>
-    <t>[{"regex":["unreachable"],"score":50},{"regex":["reachable"],"score":10}]</t>
-  </si>
-  <si>
     <t>cis_sw_int</t>
   </si>
   <si>
@@ -97,10 +94,13 @@
     <t>speed,duplex,bits,error</t>
   </si>
   <si>
-    <t>[{"regex":["down"],"score":20},{"regex":["up"],"score":0}]</t>
-  </si>
-  <si>
     <t>Fa0/1</t>
+  </si>
+  <si>
+    <t>[{"regex":["unreachable"],"score":0},{"regex":["reachable"],"score":100}]</t>
+  </si>
+  <si>
+    <t>[{"regex":["down"],"score":0},{"regex":["up"],"score":100}]</t>
   </si>
 </sst>
 </file>
@@ -931,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1024,7 @@
         <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1053,16 +1053,16 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1091,16 +1091,16 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
         <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
         <v>21</v>
       </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1167,16 +1167,16 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
         <v>23</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>24</v>
       </c>
-      <c r="K6" t="s">
-        <v>25</v>
-      </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1205,16 +1205,16 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
         <v>27</v>
-      </c>
-      <c r="K7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
         <v>21</v>
       </c>
       <c r="L8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1281,16 +1281,16 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" t="s">
         <v>23</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>24</v>
       </c>
-      <c r="K9" t="s">
-        <v>25</v>
-      </c>
       <c r="L9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1319,16 +1319,16 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" t="s">
         <v>27</v>
-      </c>
-      <c r="K10" t="s">
-        <v>25</v>
-      </c>
-      <c r="L10" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>